<commit_message>
Removed extra spaces in canevas values
</commit_message>
<xml_diff>
--- a/raphael_canevas.xlsx
+++ b/raphael_canevas.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="192">
   <si>
     <t xml:space="preserve">Encadré</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve">[2.5-17.6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AML_type</t>
   </si>
   <si>
     <t xml:space="preserve">Type of AML</t>
@@ -770,7 +773,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -778,7 +781,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,6 +1027,9 @@
       <c r="C11" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
@@ -1035,20 +1041,23 @@
       <c r="A12" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,12 +1081,12 @@
         <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
@@ -1085,7 +1094,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -1093,13 +1102,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>18</v>
@@ -1108,7 +1117,7 @@
         <v>42</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>43</v>
@@ -1116,13 +1125,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>18</v>
@@ -1131,7 +1140,7 @@
         <v>42</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>43</v>
@@ -1139,13 +1148,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>18</v>
@@ -1154,7 +1163,7 @@
         <v>42</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>43</v>
@@ -1162,13 +1171,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>18</v>
@@ -1177,7 +1186,7 @@
         <v>42</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>43</v>
@@ -1185,13 +1194,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>18</v>
@@ -1200,7 +1209,7 @@
         <v>42</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>43</v>
@@ -1208,13 +1217,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>18</v>
@@ -1223,7 +1232,7 @@
         <v>42</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>43</v>
@@ -1231,13 +1240,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>18</v>
@@ -1246,7 +1255,7 @@
         <v>42</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>43</v>
@@ -1254,13 +1263,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>18</v>
@@ -1269,7 +1278,7 @@
         <v>42</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>43</v>
@@ -1277,13 +1286,13 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>18</v>
@@ -1292,7 +1301,7 @@
         <v>42</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>43</v>
@@ -1300,13 +1309,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>18</v>
@@ -1315,7 +1324,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>43</v>
@@ -1323,13 +1332,13 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>18</v>
@@ -1338,7 +1347,7 @@
         <v>42</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>43</v>
@@ -1346,13 +1355,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>18</v>
@@ -1361,7 +1370,7 @@
         <v>42</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>43</v>
@@ -1369,13 +1378,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>18</v>
@@ -1384,7 +1393,7 @@
         <v>42</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>43</v>
@@ -1392,13 +1401,13 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>18</v>
@@ -1407,7 +1416,7 @@
         <v>42</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>43</v>
@@ -1415,13 +1424,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>18</v>
@@ -1430,7 +1439,7 @@
         <v>42</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>43</v>
@@ -1438,13 +1447,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>18</v>
@@ -1453,7 +1462,7 @@
         <v>42</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>43</v>
@@ -1461,13 +1470,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>18</v>
@@ -1476,7 +1485,7 @@
         <v>42</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>43</v>
@@ -1484,13 +1493,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>18</v>
@@ -1499,7 +1508,7 @@
         <v>42</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>43</v>
@@ -1507,13 +1516,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>18</v>
@@ -1522,7 +1531,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>43</v>
@@ -1530,13 +1539,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>18</v>
@@ -1545,7 +1554,7 @@
         <v>42</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>43</v>
@@ -1553,13 +1562,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>18</v>
@@ -1568,7 +1577,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>43</v>
@@ -1576,13 +1585,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>18</v>
@@ -1591,7 +1600,7 @@
         <v>42</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>43</v>
@@ -1599,13 +1608,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>18</v>
@@ -1614,7 +1623,7 @@
         <v>42</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>43</v>
@@ -1622,13 +1631,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>18</v>
@@ -1637,7 +1646,7 @@
         <v>42</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>43</v>
@@ -1645,13 +1654,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>18</v>
@@ -1660,7 +1669,7 @@
         <v>42</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>43</v>
@@ -1668,13 +1677,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>18</v>
@@ -1683,7 +1692,7 @@
         <v>42</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>43</v>
@@ -1691,36 +1700,36 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>18</v>
@@ -1729,7 +1738,7 @@
         <v>42</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>43</v>
@@ -1737,13 +1746,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>18</v>
@@ -1752,7 +1761,7 @@
         <v>42</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>43</v>
@@ -1760,13 +1769,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>18</v>
@@ -1775,7 +1784,7 @@
         <v>42</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>43</v>
@@ -1783,13 +1792,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>18</v>
@@ -1798,7 +1807,7 @@
         <v>42</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>43</v>
@@ -1806,13 +1815,13 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>18</v>
@@ -1821,7 +1830,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>43</v>
@@ -1829,36 +1838,36 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>18</v>
@@ -1867,7 +1876,7 @@
         <v>42</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>43</v>
@@ -1875,13 +1884,13 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>18</v>
@@ -1890,7 +1899,7 @@
         <v>42</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>43</v>
@@ -1898,10 +1907,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">B53</f>
@@ -1911,21 +1920,21 @@
         <v>18</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">B54</f>
@@ -1935,44 +1944,44 @@
         <v>18</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">B56</f>
@@ -1982,21 +1991,21 @@
         <v>18</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">B57</f>
@@ -2006,21 +2015,21 @@
         <v>18</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">B58</f>
@@ -2030,21 +2039,21 @@
         <v>18</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">B59</f>
@@ -2054,21 +2063,21 @@
         <v>18</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">B60</f>
@@ -2078,21 +2087,21 @@
         <v>18</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">B61</f>
@@ -2102,21 +2111,21 @@
         <v>18</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">B62</f>
@@ -2126,21 +2135,21 @@
         <v>18</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">B63</f>
@@ -2150,21 +2159,21 @@
         <v>18</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">B64</f>
@@ -2174,21 +2183,21 @@
         <v>18</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">B65</f>
@@ -2198,21 +2207,21 @@
         <v>18</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">B66</f>
@@ -2222,21 +2231,21 @@
         <v>18</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">B67</f>
@@ -2246,21 +2255,21 @@
         <v>18</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">B68</f>
@@ -2270,21 +2279,21 @@
         <v>18</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">B69</f>
@@ -2294,21 +2303,21 @@
         <v>18</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">B70</f>
@@ -2318,21 +2327,21 @@
         <v>18</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">B71</f>
@@ -2342,21 +2351,21 @@
         <v>18</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">B72</f>
@@ -2366,21 +2375,21 @@
         <v>18</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">B73</f>
@@ -2390,21 +2399,21 @@
         <v>18</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">B74</f>
@@ -2414,21 +2423,21 @@
         <v>18</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">B75</f>
@@ -2438,21 +2447,21 @@
         <v>18</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">B76</f>
@@ -2462,21 +2471,21 @@
         <v>18</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">B77</f>
@@ -2486,21 +2495,21 @@
         <v>18</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">B78</f>
@@ -2510,21 +2519,21 @@
         <v>18</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">B79</f>
@@ -2534,21 +2543,21 @@
         <v>18</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">B80</f>
@@ -2558,21 +2567,21 @@
         <v>18</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">B81</f>
@@ -2582,21 +2591,21 @@
         <v>18</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">B82</f>
@@ -2606,21 +2615,21 @@
         <v>18</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">B83</f>
@@ -2630,21 +2639,21 @@
         <v>18</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">B84</f>
@@ -2654,21 +2663,21 @@
         <v>18</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">B85</f>
@@ -2678,21 +2687,21 @@
         <v>18</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F85" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">B86</f>
@@ -2702,21 +2711,21 @@
         <v>18</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">B87</f>
@@ -2726,21 +2735,21 @@
         <v>18</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F87" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">B88</f>
@@ -2750,21 +2759,21 @@
         <v>18</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F88" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">B89</f>
@@ -2774,21 +2783,21 @@
         <v>18</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">B90</f>
@@ -2798,21 +2807,21 @@
         <v>18</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">B91</f>
@@ -2822,21 +2831,21 @@
         <v>18</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">B92</f>
@@ -2846,21 +2855,21 @@
         <v>18</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">B93</f>
@@ -2870,21 +2879,21 @@
         <v>18</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F93" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">B94</f>
@@ -2894,21 +2903,21 @@
         <v>18</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F94" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">B95</f>
@@ -2918,21 +2927,21 @@
         <v>18</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F95" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C96" s="0" t="str">
         <f aca="false">B96</f>
@@ -2942,21 +2951,21 @@
         <v>18</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F96" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C97" s="0" t="str">
         <f aca="false">B97</f>
@@ -2966,21 +2975,21 @@
         <v>18</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F97" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C98" s="0" t="str">
         <f aca="false">B98</f>
@@ -2990,21 +2999,21 @@
         <v>18</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C99" s="0" t="str">
         <f aca="false">B99</f>
@@ -3014,21 +3023,21 @@
         <v>18</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F99" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C100" s="0" t="str">
         <f aca="false">B100</f>
@@ -3038,62 +3047,62 @@
         <v>18</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F100" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F102" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all inputs in one dataframe when Compute button pressed
</commit_message>
<xml_diff>
--- a/raphael_canevas.xlsx
+++ b/raphael_canevas.xlsx
@@ -773,7 +773,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Prepare and transform inputs in a dataframe for analysis
</commit_message>
<xml_diff>
--- a/raphael_canevas.xlsx
+++ b/raphael_canevas.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="193">
   <si>
     <t xml:space="preserve">Encadré</t>
   </si>
@@ -212,55 +212,58 @@
     <t xml:space="preserve">Present,Absent,NA</t>
   </si>
   <si>
+    <t xml:space="preserve">1=Present,0=Absent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HB_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HB (U/H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2.5-17.6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AML_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of AML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de novo,secondary,therapy-related,other,N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de novo : oAML==0,tAML==0,sAML==0 ; secondary : oAML==0,tAML==0,sAML==1; therapy-related:  oAML==0,tAML==1,sAML==0 ; other:  oAML==1,tAML==0,sAML==0; N/A : oAML==NA,tAML==NA,sAML==NA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oAML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tAML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sAML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transplantCR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transplantRel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytogenetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv16_t16_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv(16) or t(16;16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absent</t>
+  </si>
+  <si>
     <t xml:space="preserve">1=Present,0=absent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HB_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HB (U/H)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[2.5-17.6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AML_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of AML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de novo,secondary,therapy-related,other,N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de novo : oAML==0,tAML==0,sAML==0 ; secondary : oAML==0,tAML==0,sAML==1; therapy-related:  oAML==0,tAML==1,sAML==0 ; other:  oAML==1,tAML==0,sAML==0; N/A : oAML==NA,tAML==NA,sAML==NA. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">oAML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tAML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sAML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transplantCR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transplantRel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytogenetics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv16_t16_16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv(16) or t(16;16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absent</t>
   </si>
   <si>
     <t xml:space="preserve">t_15_17</t>
@@ -772,8 +775,8 @@
   </sheetPr>
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1120,7 +1123,7 @@
         <v>59</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,10 +1131,10 @@
         <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>18</v>
@@ -1143,7 +1146,7 @@
         <v>59</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,10 +1154,10 @@
         <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>18</v>
@@ -1166,7 +1169,7 @@
         <v>59</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,10 +1177,10 @@
         <v>56</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>18</v>
@@ -1189,7 +1192,7 @@
         <v>59</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,10 +1200,10 @@
         <v>56</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>18</v>
@@ -1212,7 +1215,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,10 +1223,10 @@
         <v>56</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>18</v>
@@ -1235,7 +1238,7 @@
         <v>59</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,10 +1246,10 @@
         <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>18</v>
@@ -1258,7 +1261,7 @@
         <v>59</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,10 +1269,10 @@
         <v>56</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>18</v>
@@ -1281,7 +1284,7 @@
         <v>59</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,10 +1292,10 @@
         <v>56</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>18</v>
@@ -1304,7 +1307,7 @@
         <v>59</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,10 +1315,10 @@
         <v>56</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>18</v>
@@ -1327,7 +1330,7 @@
         <v>59</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,10 +1338,10 @@
         <v>56</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>18</v>
@@ -1350,7 +1353,7 @@
         <v>59</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,10 +1361,10 @@
         <v>56</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>18</v>
@@ -1373,7 +1376,7 @@
         <v>59</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,10 +1384,10 @@
         <v>56</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>18</v>
@@ -1396,7 +1399,7 @@
         <v>59</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,10 +1407,10 @@
         <v>56</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>18</v>
@@ -1419,7 +1422,7 @@
         <v>59</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,10 +1430,10 @@
         <v>56</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>18</v>
@@ -1442,7 +1445,7 @@
         <v>59</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,10 +1453,10 @@
         <v>56</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>18</v>
@@ -1465,7 +1468,7 @@
         <v>59</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,10 +1476,10 @@
         <v>56</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>18</v>
@@ -1488,7 +1491,7 @@
         <v>59</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,10 +1499,10 @@
         <v>56</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>18</v>
@@ -1511,7 +1514,7 @@
         <v>59</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,10 +1522,10 @@
         <v>56</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>18</v>
@@ -1534,7 +1537,7 @@
         <v>59</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,10 +1545,10 @@
         <v>56</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>18</v>
@@ -1557,7 +1560,7 @@
         <v>59</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,10 +1568,10 @@
         <v>56</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>18</v>
@@ -1580,7 +1583,7 @@
         <v>59</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,10 +1591,10 @@
         <v>56</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>18</v>
@@ -1603,7 +1606,7 @@
         <v>59</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,10 +1614,10 @@
         <v>56</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>18</v>
@@ -1626,7 +1629,7 @@
         <v>59</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,10 +1637,10 @@
         <v>56</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>18</v>
@@ -1649,7 +1652,7 @@
         <v>59</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,10 +1660,10 @@
         <v>56</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>18</v>
@@ -1672,7 +1675,7 @@
         <v>59</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,10 +1683,10 @@
         <v>56</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>18</v>
@@ -1695,41 +1698,41 @@
         <v>59</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>18</v>
@@ -1741,18 +1744,18 @@
         <v>59</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>18</v>
@@ -1764,18 +1767,18 @@
         <v>59</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>18</v>
@@ -1787,18 +1790,18 @@
         <v>59</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>18</v>
@@ -1810,18 +1813,18 @@
         <v>59</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>18</v>
@@ -1833,41 +1836,41 @@
         <v>59</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>18</v>
@@ -1879,18 +1882,18 @@
         <v>59</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>18</v>
@@ -1902,15 +1905,15 @@
         <v>59</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">B53</f>
@@ -1920,21 +1923,21 @@
         <v>18</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">B54</f>
@@ -1944,44 +1947,44 @@
         <v>18</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">B56</f>
@@ -1991,21 +1994,21 @@
         <v>18</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">B57</f>
@@ -2015,21 +2018,21 @@
         <v>18</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">B58</f>
@@ -2039,21 +2042,21 @@
         <v>18</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">B59</f>
@@ -2063,21 +2066,21 @@
         <v>18</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">B60</f>
@@ -2087,21 +2090,21 @@
         <v>18</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">B61</f>
@@ -2111,21 +2114,21 @@
         <v>18</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">B62</f>
@@ -2135,21 +2138,21 @@
         <v>18</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">B63</f>
@@ -2159,21 +2162,21 @@
         <v>18</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">B64</f>
@@ -2183,21 +2186,21 @@
         <v>18</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">B65</f>
@@ -2207,21 +2210,21 @@
         <v>18</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">B66</f>
@@ -2231,21 +2234,21 @@
         <v>18</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">B67</f>
@@ -2255,21 +2258,21 @@
         <v>18</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">B68</f>
@@ -2279,21 +2282,21 @@
         <v>18</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">B69</f>
@@ -2303,21 +2306,21 @@
         <v>18</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">B70</f>
@@ -2327,21 +2330,21 @@
         <v>18</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">B71</f>
@@ -2351,21 +2354,21 @@
         <v>18</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">B72</f>
@@ -2375,21 +2378,21 @@
         <v>18</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">B73</f>
@@ -2399,21 +2402,21 @@
         <v>18</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">B74</f>
@@ -2423,21 +2426,21 @@
         <v>18</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">B75</f>
@@ -2447,21 +2450,21 @@
         <v>18</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">B76</f>
@@ -2471,21 +2474,21 @@
         <v>18</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">B77</f>
@@ -2495,21 +2498,21 @@
         <v>18</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">B78</f>
@@ -2519,21 +2522,21 @@
         <v>18</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">B79</f>
@@ -2543,21 +2546,21 @@
         <v>18</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">B80</f>
@@ -2567,21 +2570,21 @@
         <v>18</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">B81</f>
@@ -2591,21 +2594,21 @@
         <v>18</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">B82</f>
@@ -2615,21 +2618,21 @@
         <v>18</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">B83</f>
@@ -2639,21 +2642,21 @@
         <v>18</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">B84</f>
@@ -2663,21 +2666,21 @@
         <v>18</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">B85</f>
@@ -2687,21 +2690,21 @@
         <v>18</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F85" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">B86</f>
@@ -2711,21 +2714,21 @@
         <v>18</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">B87</f>
@@ -2735,21 +2738,21 @@
         <v>18</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F87" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">B88</f>
@@ -2759,21 +2762,21 @@
         <v>18</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F88" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">B89</f>
@@ -2783,21 +2786,21 @@
         <v>18</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">B90</f>
@@ -2807,21 +2810,21 @@
         <v>18</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">B91</f>
@@ -2831,21 +2834,21 @@
         <v>18</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">B92</f>
@@ -2855,21 +2858,21 @@
         <v>18</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">B93</f>
@@ -2879,21 +2882,21 @@
         <v>18</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F93" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">B94</f>
@@ -2903,21 +2906,21 @@
         <v>18</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F94" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">B95</f>
@@ -2927,21 +2930,21 @@
         <v>18</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F95" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C96" s="0" t="str">
         <f aca="false">B96</f>
@@ -2951,21 +2954,21 @@
         <v>18</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F96" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C97" s="0" t="str">
         <f aca="false">B97</f>
@@ -2975,21 +2978,21 @@
         <v>18</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F97" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C98" s="0" t="str">
         <f aca="false">B98</f>
@@ -2999,21 +3002,21 @@
         <v>18</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C99" s="0" t="str">
         <f aca="false">B99</f>
@@ -3023,21 +3026,21 @@
         <v>18</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F99" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C100" s="0" t="str">
         <f aca="false">B100</f>
@@ -3047,62 +3050,62 @@
         <v>18</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F100" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F102" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added gerstung score and HSCT prediction
</commit_message>
<xml_diff>
--- a/raphael_canevas.xlsx
+++ b/raphael_canevas.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="194">
   <si>
     <t xml:space="preserve">Encadré</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t xml:space="preserve">ASXL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATRX</t>
   </si>
   <si>
     <t xml:space="preserve">RUNX1</t>
@@ -773,10 +776,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1932,16 +1935,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>111</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="0" t="str">
-        <f aca="false">B54</f>
-        <v>RUNX1</v>
+      <c r="C54" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>18</v>
@@ -1963,8 +1965,9 @@
       <c r="B55" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>133</v>
+      <c r="C55" s="0" t="str">
+        <f aca="false">B55</f>
+        <v>RUNX1</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>18</v>
@@ -1981,14 +1984,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C56" s="0" t="str">
-        <f aca="false">B56</f>
-        <v>BCOR</v>
+      <c r="C56" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>18</v>
@@ -2005,14 +2007,14 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>136</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">B57</f>
-        <v>BRAF</v>
+        <v>BCOR</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>18</v>
@@ -2029,14 +2031,14 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>137</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">B58</f>
-        <v>CBL</v>
+        <v>BRAF</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>18</v>
@@ -2053,14 +2055,14 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">B59</f>
-        <v>DNMT3A</v>
+        <v>CBL</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>18</v>
@@ -2077,14 +2079,14 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">B60</f>
-        <v>ETV6</v>
+        <v>DNMT3A</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>18</v>
@@ -2101,14 +2103,14 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>140</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">B61</f>
-        <v>EZH2</v>
+        <v>ETV6</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>18</v>
@@ -2125,14 +2127,14 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>141</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">B62</f>
-        <v>GATA2</v>
+        <v>EZH2</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>18</v>
@@ -2149,14 +2151,14 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>142</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">B63</f>
-        <v>JAK2</v>
+        <v>GATA2</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>18</v>
@@ -2173,14 +2175,14 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>143</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">B64</f>
-        <v>KIT</v>
+        <v>JAK2</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>18</v>
@@ -2197,14 +2199,14 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>144</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">B65</f>
-        <v>KRAS</v>
+        <v>KIT</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>18</v>
@@ -2221,14 +2223,14 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>145</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">B66</f>
-        <v>MPL</v>
+        <v>KRAS</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>18</v>
@@ -2245,14 +2247,14 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>146</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">B67</f>
-        <v>NF1</v>
+        <v>MPL</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>18</v>
@@ -2269,14 +2271,14 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>147</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">B68</f>
-        <v>NRAS</v>
+        <v>NF1</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>18</v>
@@ -2293,14 +2295,14 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>148</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">B69</f>
-        <v>PHF6</v>
+        <v>NRAS</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>18</v>
@@ -2317,14 +2319,14 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>149</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">B70</f>
-        <v>PTPN11</v>
+        <v>PHF6</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>18</v>
@@ -2341,14 +2343,14 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>150</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">B71</f>
-        <v>RAD21</v>
+        <v>PTPN11</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>18</v>
@@ -2365,14 +2367,14 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>151</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">B72</f>
-        <v>SF3B1</v>
+        <v>RAD21</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>18</v>
@@ -2389,14 +2391,14 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>152</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">B73</f>
-        <v>SFRS2</v>
+        <v>SF3B1</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>18</v>
@@ -2413,14 +2415,14 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>153</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">B74</f>
-        <v>STAG2</v>
+        <v>SFRS2</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>18</v>
@@ -2437,14 +2439,14 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>154</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">B75</f>
-        <v>TET2</v>
+        <v>STAG2</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>18</v>
@@ -2461,14 +2463,14 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>155</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">B76</f>
-        <v>U2AF1</v>
+        <v>TET2</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>18</v>
@@ -2485,14 +2487,14 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>156</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">B77</f>
-        <v>WT1</v>
+        <v>U2AF1</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>18</v>
@@ -2509,14 +2511,14 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>157</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">B78</f>
-        <v>ZRSR2</v>
+        <v>WT1</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>18</v>
@@ -2533,14 +2535,14 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>159</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">B79</f>
-        <v>CBLB</v>
+        <v>ZRSR2</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>18</v>
@@ -2549,7 +2551,7 @@
         <v>113</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="G79" s="0" t="s">
         <v>115</v>
@@ -2557,14 +2559,14 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>160</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">B80</f>
-        <v>CDKN2A</v>
+        <v>CBLB</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>18</v>
@@ -2581,14 +2583,14 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>161</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">B81</f>
-        <v>CREBBP</v>
+        <v>CDKN2A</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>18</v>
@@ -2605,14 +2607,14 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>162</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">B82</f>
-        <v>CUX1</v>
+        <v>CREBBP</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>18</v>
@@ -2629,14 +2631,14 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>163</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">B83</f>
-        <v>EP300</v>
+        <v>CUX1</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>18</v>
@@ -2653,14 +2655,14 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">B84</f>
-        <v>FBXW7</v>
+        <v>EP300</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>18</v>
@@ -2677,14 +2679,14 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>165</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">B85</f>
-        <v>GNAS</v>
+        <v>FBXW7</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>18</v>
@@ -2701,14 +2703,14 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>166</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">B86</f>
-        <v>IKZF1</v>
+        <v>GNAS</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>18</v>
@@ -2725,14 +2727,14 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>167</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">B87</f>
-        <v>KDM5A</v>
+        <v>IKZF1</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>18</v>
@@ -2749,14 +2751,14 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>168</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">B88</f>
-        <v>KDM6A</v>
+        <v>KDM5A</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>18</v>
@@ -2773,14 +2775,14 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>169</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">B89</f>
-        <v>MLL</v>
+        <v>KDM6A</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>18</v>
@@ -2797,14 +2799,14 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>170</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">B90</f>
-        <v>MLL2</v>
+        <v>MLL</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>18</v>
@@ -2821,14 +2823,14 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>171</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">B91</f>
-        <v>MLL3</v>
+        <v>MLL2</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>18</v>
@@ -2845,14 +2847,14 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>172</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">B92</f>
-        <v>MLL5</v>
+        <v>MLL3</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>18</v>
@@ -2869,14 +2871,14 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>173</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">B93</f>
-        <v>MYC</v>
+        <v>MLL5</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>18</v>
@@ -2893,14 +2895,14 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>174</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">B94</f>
-        <v>PRPF40B</v>
+        <v>MYC</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>18</v>
@@ -2917,14 +2919,14 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>175</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">B95</f>
-        <v>PTEN</v>
+        <v>PRPF40B</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>18</v>
@@ -2941,14 +2943,14 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>176</v>
       </c>
       <c r="C96" s="0" t="str">
         <f aca="false">B96</f>
-        <v>RB1</v>
+        <v>PTEN</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>18</v>
@@ -2965,14 +2967,14 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>177</v>
       </c>
       <c r="C97" s="0" t="str">
         <f aca="false">B97</f>
-        <v>SF1</v>
+        <v>RB1</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>18</v>
@@ -2989,14 +2991,14 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>178</v>
       </c>
       <c r="C98" s="0" t="str">
         <f aca="false">B98</f>
-        <v>SF3A1</v>
+        <v>SF1</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>18</v>
@@ -3013,14 +3015,14 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>179</v>
       </c>
       <c r="C99" s="0" t="str">
         <f aca="false">B99</f>
-        <v>SH2B3</v>
+        <v>SF3A1</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>18</v>
@@ -3037,14 +3039,14 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>180</v>
       </c>
       <c r="C100" s="0" t="str">
         <f aca="false">B100</f>
-        <v>U2AF2</v>
+        <v>SH2B3</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>18</v>
@@ -3061,51 +3063,75 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B101" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>183</v>
+      <c r="C101" s="0" t="str">
+        <f aca="false">B101</f>
+        <v>U2AF2</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G102" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B102" s="0" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="B103" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D102" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="C103" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="F102" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G102" s="0" t="s">
+      <c r="D103" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="I102" s="0" t="s">
+      <c r="F103" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" s="0" t="s">
         <v>192</v>
+      </c>
+      <c r="I103" s="0" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>